<commit_message>
throne template prism wording
</commit_message>
<xml_diff>
--- a/assets/Throne Template.xlsx
+++ b/assets/Throne Template.xlsx
@@ -22,19 +22,19 @@
     <t>Focus</t>
   </si>
   <si>
-    <t>Prism Formation 1</t>
+    <t>Prism Formation Top 1</t>
   </si>
   <si>
-    <t>Prism Formation 2</t>
+    <t>Prism Formation Right 1</t>
   </si>
   <si>
     <t>FastForward</t>
   </si>
   <si>
-    <t>Prism Formation 3</t>
+    <t>Prism Formation Top 2</t>
   </si>
   <si>
-    <t>Prism Formation 4</t>
+    <t>Prism Formation Right 2</t>
   </si>
   <si>
     <t>Rewind</t>
@@ -46,10 +46,10 @@
     <t>Wait</t>
   </si>
   <si>
-    <t>Prism Formation 1&amp;2</t>
+    <t>Prism Formation Top 1&amp;2</t>
   </si>
   <si>
-    <t>Prism Formation 3&amp;4</t>
+    <t>Prism Formation Right 3&amp;4</t>
   </si>
 </sst>
 </file>
@@ -87,16 +87,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <right/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -117,9 +114,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -143,7 +137,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.14"/>
+    <col customWidth="1" min="2" max="2" width="23.14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -367,7 +361,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -375,7 +369,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
@@ -687,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -695,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -1007,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109">
@@ -1015,7 +1009,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110">
@@ -1327,7 +1321,7 @@
         <v>2</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149">
@@ -1335,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="150">
@@ -1647,7 +1641,7 @@
         <v>2</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189">
@@ -1655,7 +1649,7 @@
         <v>2</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="190">
@@ -1774,7 +1768,7 @@
       <c r="A204" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B204" s="5" t="s">
+      <c r="B204" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1782,7 +1776,7 @@
       <c r="A205" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B205" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1790,7 +1784,7 @@
       <c r="A206" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B206" s="4" t="s">
+      <c r="B206" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1798,7 +1792,7 @@
       <c r="A207" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B207" s="5" t="s">
+      <c r="B207" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1806,7 +1800,7 @@
       <c r="A208" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="B208" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1814,7 +1808,7 @@
       <c r="A209" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B209" s="4" t="s">
+      <c r="B209" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1822,7 +1816,7 @@
       <c r="A210" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B210" s="4" t="s">
+      <c r="B210" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1830,7 +1824,7 @@
       <c r="A211" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B211" s="4" t="s">
+      <c r="B211" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1838,7 +1832,7 @@
       <c r="A212" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B212" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1846,7 +1840,7 @@
       <c r="A213" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B213" s="4" t="s">
+      <c r="B213" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1854,7 +1848,7 @@
       <c r="A214" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B214" s="5" t="s">
+      <c r="B214" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1862,7 +1856,7 @@
       <c r="A215" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B215" s="4" t="s">
+      <c r="B215" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1870,7 +1864,7 @@
       <c r="A216" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B216" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1878,7 +1872,7 @@
       <c r="A217" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B217" s="5" t="s">
+      <c r="B217" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1886,7 +1880,7 @@
       <c r="A218" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B218" s="4" t="s">
+      <c r="B218" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1894,7 +1888,7 @@
       <c r="A219" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B219" s="4" t="s">
+      <c r="B219" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1902,7 +1896,7 @@
       <c r="A220" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B220" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1910,7 +1904,7 @@
       <c r="A221" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B221" s="4" t="s">
+      <c r="B221" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1918,7 +1912,7 @@
       <c r="A222" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="B222" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1926,7 +1920,7 @@
       <c r="A223" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B223" s="4" t="s">
+      <c r="B223" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1934,7 +1928,7 @@
       <c r="A224" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B224" s="4" t="s">
+      <c r="B224" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1942,7 +1936,7 @@
       <c r="A225" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B225" s="4" t="s">
+      <c r="B225" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1950,7 +1944,7 @@
       <c r="A226" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B226" s="4" t="s">
+      <c r="B226" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1958,7 +1952,7 @@
       <c r="A227" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B227" s="5" t="s">
+      <c r="B227" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1966,23 +1960,23 @@
       <c r="A228" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B228" s="5" t="s">
-        <v>4</v>
+      <c r="B228" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B229" s="5" t="s">
-        <v>6</v>
+      <c r="B229" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B230" s="5" t="s">
+      <c r="B230" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1990,7 +1984,7 @@
       <c r="A231" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B231" s="4" t="s">
+      <c r="B231" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1998,7 +1992,7 @@
       <c r="A232" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B232" s="4" t="s">
+      <c r="B232" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2006,7 +2000,7 @@
       <c r="A233" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B233" s="7" t="s">
+      <c r="B233" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2014,7 +2008,7 @@
       <c r="A234" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B234" s="4" t="s">
+      <c r="B234" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2022,7 +2016,7 @@
       <c r="A235" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B235" s="7" t="s">
+      <c r="B235" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2094,7 +2088,7 @@
       <c r="A244" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B244" s="5" t="s">
+      <c r="B244" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2102,7 +2096,7 @@
       <c r="A245" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B245" s="4" t="s">
+      <c r="B245" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2110,7 +2104,7 @@
       <c r="A246" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B246" s="4" t="s">
+      <c r="B246" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2118,7 +2112,7 @@
       <c r="A247" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B247" s="5" t="s">
+      <c r="B247" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2126,7 +2120,7 @@
       <c r="A248" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B248" s="4" t="s">
+      <c r="B248" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2134,7 +2128,7 @@
       <c r="A249" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B249" s="4" t="s">
+      <c r="B249" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2142,7 +2136,7 @@
       <c r="A250" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B250" s="4" t="s">
+      <c r="B250" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2150,7 +2144,7 @@
       <c r="A251" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B251" s="4" t="s">
+      <c r="B251" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2158,7 +2152,7 @@
       <c r="A252" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B252" s="4" t="s">
+      <c r="B252" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2166,7 +2160,7 @@
       <c r="A253" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B253" s="4" t="s">
+      <c r="B253" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2174,7 +2168,7 @@
       <c r="A254" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B254" s="5" t="s">
+      <c r="B254" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2182,7 +2176,7 @@
       <c r="A255" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B255" s="4" t="s">
+      <c r="B255" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2190,7 +2184,7 @@
       <c r="A256" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B256" s="4" t="s">
+      <c r="B256" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2198,7 +2192,7 @@
       <c r="A257" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B257" s="5" t="s">
+      <c r="B257" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2206,7 +2200,7 @@
       <c r="A258" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B258" s="4" t="s">
+      <c r="B258" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2214,7 +2208,7 @@
       <c r="A259" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B259" s="4" t="s">
+      <c r="B259" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2222,7 +2216,7 @@
       <c r="A260" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B260" s="4" t="s">
+      <c r="B260" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2230,7 +2224,7 @@
       <c r="A261" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B261" s="4" t="s">
+      <c r="B261" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2238,7 +2232,7 @@
       <c r="A262" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B262" s="4" t="s">
+      <c r="B262" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2246,7 +2240,7 @@
       <c r="A263" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B263" s="4" t="s">
+      <c r="B263" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2254,7 +2248,7 @@
       <c r="A264" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B264" s="4" t="s">
+      <c r="B264" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2262,7 +2256,7 @@
       <c r="A265" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B265" s="4" t="s">
+      <c r="B265" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2270,7 +2264,7 @@
       <c r="A266" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B266" s="4" t="s">
+      <c r="B266" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2278,7 +2272,7 @@
       <c r="A267" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B267" s="5" t="s">
+      <c r="B267" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2286,23 +2280,23 @@
       <c r="A268" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B268" s="5" t="s">
-        <v>4</v>
+      <c r="B268" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B269" s="5" t="s">
-        <v>6</v>
+      <c r="B269" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B270" s="5" t="s">
+      <c r="B270" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2310,7 +2304,7 @@
       <c r="A271" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B271" s="4" t="s">
+      <c r="B271" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2318,7 +2312,7 @@
       <c r="A272" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B272" s="4" t="s">
+      <c r="B272" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2326,7 +2320,7 @@
       <c r="A273" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B273" s="7" t="s">
+      <c r="B273" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2334,7 +2328,7 @@
       <c r="A274" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B274" s="4" t="s">
+      <c r="B274" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2342,7 +2336,7 @@
       <c r="A275" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B275" s="7" t="s">
+      <c r="B275" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2414,7 +2408,7 @@
       <c r="A284" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B284" s="5" t="s">
+      <c r="B284" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2422,7 +2416,7 @@
       <c r="A285" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B285" s="4" t="s">
+      <c r="B285" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2430,7 +2424,7 @@
       <c r="A286" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B286" s="4" t="s">
+      <c r="B286" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2438,7 +2432,7 @@
       <c r="A287" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B287" s="5" t="s">
+      <c r="B287" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2446,7 +2440,7 @@
       <c r="A288" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B288" s="4" t="s">
+      <c r="B288" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2454,7 +2448,7 @@
       <c r="A289" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B289" s="4" t="s">
+      <c r="B289" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2462,7 +2456,7 @@
       <c r="A290" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B290" s="4" t="s">
+      <c r="B290" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2470,7 +2464,7 @@
       <c r="A291" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B291" s="4" t="s">
+      <c r="B291" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2478,7 +2472,7 @@
       <c r="A292" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B292" s="4" t="s">
+      <c r="B292" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2486,7 +2480,7 @@
       <c r="A293" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B293" s="4" t="s">
+      <c r="B293" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2494,7 +2488,7 @@
       <c r="A294" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B294" s="5" t="s">
+      <c r="B294" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2502,7 +2496,7 @@
       <c r="A295" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B295" s="4" t="s">
+      <c r="B295" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2510,7 +2504,7 @@
       <c r="A296" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B296" s="4" t="s">
+      <c r="B296" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2518,7 +2512,7 @@
       <c r="A297" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B297" s="5" t="s">
+      <c r="B297" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2526,7 +2520,7 @@
       <c r="A298" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B298" s="4" t="s">
+      <c r="B298" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2534,7 +2528,7 @@
       <c r="A299" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B299" s="4" t="s">
+      <c r="B299" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -2542,7 +2536,7 @@
       <c r="A300" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B300" s="4" t="s">
+      <c r="B300" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>